<commit_message>
this lets it see the curnt date
</commit_message>
<xml_diff>
--- a/bird_data.xlsx
+++ b/bird_data.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,81 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Bird</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>When</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>kiwi</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>50 hicks rd</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20/8/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>kiwi</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>airstrip</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>21/8/2025</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
done for night fix all the bugs i found wh  fionn tested
</commit_message>
<xml_diff>
--- a/bird_data.xlsx
+++ b/bird_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>When</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -476,6 +481,7 @@
           <t>20/8/2025</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -498,6 +504,130 @@
           <t>21/8/2025</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>kiwi</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>50 hicjs road</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-08-21 12:07:21</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>kiwi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>mill creek</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-08-21 13:20:05</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>it was small</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>kiwi</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>back road</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-08-21 13:23:56</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>haast eagle</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>mountain range</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-08-21 19:16:02</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>it was quite large</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>kiwi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>50 hicks road</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-08-21 19:26:29</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
alex tests finds problem
</commit_message>
<xml_diff>
--- a/bird_data.xlsx
+++ b/bird_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,38 +473,46 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>50 hicks rd</t>
+          <t>port willan</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>20/8/2025</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>2025-08-22 14:04:24</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>big</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>kiwi</t>
+          <t>bellbird</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>airstrip</t>
+          <t>sbhs</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>21/8/2025</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>2025-08-22 14:07:58</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>breeding pair</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,120 +522,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>50 hicjs road</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-08-21 12:07:21</t>
+          <t>2025-08-22 14:09:08</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>kiwi</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>mill creek</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2025-08-21 13:20:05</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>it was small</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>kiwi</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>back road</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2025-08-21 13:23:56</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>haast eagle</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>mountain range</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2025-08-21 19:16:02</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>it was quite large</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>kiwi</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>50 hicks road</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2025-08-21 19:26:29</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>